<commit_message>
Bulk criteria approval fixation
</commit_message>
<xml_diff>
--- a/AIS/wwwroot/Images/Page ID.xlsx
+++ b/AIS/wwwroot/Images/Page ID.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asad Ali\Documents\GitHub\IAS-VAPT\AIS\wwwroot\Images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IAS\HTTPS-IAS-Production\AIS\wwwroot\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2112" uniqueCount="925">
   <si>
     <t>PAGE_NAME</t>
   </si>
@@ -2794,6 +2794,15 @@
   </si>
   <si>
     <t>FADRiskControlPanel/Index</t>
+  </si>
+  <si>
+    <t>System Logs</t>
+  </si>
+  <si>
+    <t>AdministrationPanel/SystemLogs</t>
+  </si>
+  <si>
+    <t>SystemLogs</t>
   </si>
 </sst>
 </file>
@@ -3128,10 +3137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K299"/>
+  <dimension ref="A1:K300"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
-      <selection activeCell="F293" sqref="F293"/>
+      <selection activeCell="A306" sqref="A306:XFD306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -13029,6 +13038,38 @@
       </c>
       <c r="K299" s="1" t="s">
         <v>919</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A300" s="1">
+        <v>394</v>
+      </c>
+      <c r="B300" s="1">
+        <v>394</v>
+      </c>
+      <c r="C300" s="1">
+        <v>10</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="F300" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="G300" s="1">
+        <v>7</v>
+      </c>
+      <c r="H300" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="I300" s="1">
+        <v>0</v>
+      </c>
+      <c r="K300" s="1" t="s">
+        <v>924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>